<commit_message>
Added repository interface & added some tests
</commit_message>
<xml_diff>
--- a/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
+++ b/Docs/Lab03/Lab03_WBT_TCs_Form.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\VVSS\VVSS\Docs\Lab03\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FDC5974-DD17-4FD6-A38C-D1266879B5A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D134FF5F-891E-4F6D-8D87-435A57DDD825}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="12975" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Statement" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="224" uniqueCount="138">
   <si>
     <t>VVSS, Info Romana, 2024-2025</t>
   </si>
@@ -326,9 +326,6 @@
     <t>list1, "1part"</t>
   </si>
   <si>
-    <t>Product {id: 1, name: "1part"}</t>
-  </si>
-  <si>
     <t>1, 2, 3, 4, 5, 6, 7, 8, 2, 9, 11, 12</t>
   </si>
   <si>
@@ -341,9 +338,6 @@
     <t>list1,  "2"</t>
   </si>
   <si>
-    <t>Product {id: 2, name: "2"}</t>
-  </si>
-  <si>
     <t>1, 2, 3, 4, 5, 6, 7, 2, 9, 11, 12</t>
   </si>
   <si>
@@ -351,9 +345,6 @@
   </si>
   <si>
     <t>list1, "pa"</t>
-  </si>
-  <si>
-    <t>Product{id: 3, name: "3part"}</t>
   </si>
   <si>
     <t>1, 2, 3, 4, 5, 7, 2, 9, 11, 12</t>
@@ -1632,16 +1623,6 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1658,18 +1639,15 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1678,6 +1656,7 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="11" fillId="4" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1687,27 +1666,71 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="11" fillId="6" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1724,47 +1747,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="10" borderId="35" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="39" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2974,7 +2965,9 @@
   </sheetPr>
   <dimension ref="B1:Q1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
   <cols>
@@ -4110,8 +4103,8 @@
   </sheetPr>
   <dimension ref="B1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14:P15"/>
+    <sheetView topLeftCell="A7" zoomScale="75" workbookViewId="0">
+      <selection activeCell="P17" sqref="P17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -4138,7 +4131,7 @@
     </row>
     <row r="2" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="47" t="s">
+      <c r="B3" s="60" t="s">
         <v>19</v>
       </c>
       <c r="C3" s="44"/>
@@ -4170,20 +4163,20 @@
       <c r="L6" s="44"/>
       <c r="M6" s="44"/>
       <c r="N6" s="44"/>
-      <c r="O6" s="48"/>
+      <c r="O6" s="57"/>
       <c r="Q6" s="43" t="s">
         <v>22</v>
       </c>
       <c r="R6" s="44"/>
       <c r="S6" s="44"/>
-      <c r="T6" s="48"/>
+      <c r="T6" s="57"/>
     </row>
     <row r="7" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="8" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="C8" s="49" t="s">
+      <c r="C8" s="58" t="s">
         <v>24</v>
       </c>
       <c r="D8" s="44"/>
@@ -4193,7 +4186,7 @@
       <c r="I8" s="1" t="s">
         <v>25</v>
       </c>
-      <c r="Q8" s="51" t="s">
+      <c r="Q8" s="47" t="s">
         <v>26</v>
       </c>
       <c r="R8" s="44"/>
@@ -4206,7 +4199,7 @@
       <c r="B9" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="C9" s="46" t="s">
+      <c r="C9" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D9" s="44"/>
@@ -4214,7 +4207,7 @@
       <c r="F9" s="14"/>
       <c r="G9" s="14"/>
       <c r="I9" s="15"/>
-      <c r="Q9" s="51" t="s">
+      <c r="Q9" s="47" t="s">
         <v>29</v>
       </c>
       <c r="R9" s="44"/>
@@ -4227,23 +4220,23 @@
       <c r="B10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D10" s="44"/>
       <c r="E10" s="45"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>
-      <c r="I10" s="52" t="s">
+      <c r="I10" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J10" s="53"/>
-      <c r="K10" s="53"/>
-      <c r="L10" s="53"/>
-      <c r="M10" s="53"/>
-      <c r="N10" s="53"/>
-      <c r="O10" s="54"/>
-      <c r="Q10" s="51" t="s">
+      <c r="J10" s="49"/>
+      <c r="K10" s="49"/>
+      <c r="L10" s="49"/>
+      <c r="M10" s="49"/>
+      <c r="N10" s="49"/>
+      <c r="O10" s="50"/>
+      <c r="Q10" s="47" t="s">
         <v>33</v>
       </c>
       <c r="R10" s="44"/>
@@ -4256,229 +4249,229 @@
       <c r="B11" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="C11" s="46" t="s">
+      <c r="C11" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D11" s="44"/>
       <c r="E11" s="45"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="I11" s="55"/>
-      <c r="J11" s="56"/>
-      <c r="K11" s="56"/>
-      <c r="L11" s="56"/>
-      <c r="M11" s="56"/>
-      <c r="N11" s="56"/>
-      <c r="O11" s="57"/>
+      <c r="I11" s="51"/>
+      <c r="J11" s="52"/>
+      <c r="K11" s="52"/>
+      <c r="L11" s="52"/>
+      <c r="M11" s="52"/>
+      <c r="N11" s="52"/>
+      <c r="O11" s="53"/>
     </row>
     <row r="12" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C12" s="46" t="s">
+      <c r="C12" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D12" s="44"/>
       <c r="E12" s="45"/>
       <c r="F12" s="14"/>
       <c r="G12" s="14"/>
-      <c r="I12" s="55"/>
-      <c r="J12" s="56"/>
-      <c r="K12" s="56"/>
-      <c r="L12" s="56"/>
-      <c r="M12" s="56"/>
-      <c r="N12" s="56"/>
-      <c r="O12" s="57"/>
+      <c r="I12" s="51"/>
+      <c r="J12" s="52"/>
+      <c r="K12" s="52"/>
+      <c r="L12" s="52"/>
+      <c r="M12" s="52"/>
+      <c r="N12" s="52"/>
+      <c r="O12" s="53"/>
     </row>
     <row r="13" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="C13" s="46" t="s">
+      <c r="C13" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D13" s="44"/>
       <c r="E13" s="45"/>
       <c r="F13" s="14"/>
       <c r="G13" s="14"/>
-      <c r="I13" s="55"/>
-      <c r="J13" s="56"/>
-      <c r="K13" s="56"/>
-      <c r="L13" s="56"/>
-      <c r="M13" s="56"/>
-      <c r="N13" s="56"/>
-      <c r="O13" s="57"/>
+      <c r="I13" s="51"/>
+      <c r="J13" s="52"/>
+      <c r="K13" s="52"/>
+      <c r="L13" s="52"/>
+      <c r="M13" s="52"/>
+      <c r="N13" s="52"/>
+      <c r="O13" s="53"/>
       <c r="Q13" s="43" t="s">
         <v>38</v>
       </c>
       <c r="R13" s="44"/>
       <c r="S13" s="44"/>
-      <c r="T13" s="48"/>
+      <c r="T13" s="57"/>
     </row>
     <row r="14" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="5" t="s">
         <v>36</v>
       </c>
-      <c r="C14" s="46" t="s">
+      <c r="C14" s="59" t="s">
         <v>28</v>
       </c>
       <c r="D14" s="44"/>
       <c r="E14" s="45"/>
       <c r="F14" s="14"/>
       <c r="G14" s="14"/>
-      <c r="I14" s="55"/>
-      <c r="J14" s="56"/>
-      <c r="K14" s="56"/>
-      <c r="L14" s="56"/>
-      <c r="M14" s="56"/>
-      <c r="N14" s="56"/>
-      <c r="O14" s="57"/>
+      <c r="I14" s="51"/>
+      <c r="J14" s="52"/>
+      <c r="K14" s="52"/>
+      <c r="L14" s="52"/>
+      <c r="M14" s="52"/>
+      <c r="N14" s="52"/>
+      <c r="O14" s="53"/>
     </row>
     <row r="15" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I15" s="55"/>
-      <c r="J15" s="56"/>
-      <c r="K15" s="56"/>
-      <c r="L15" s="56"/>
-      <c r="M15" s="56"/>
-      <c r="N15" s="56"/>
-      <c r="O15" s="57"/>
+      <c r="I15" s="51"/>
+      <c r="J15" s="52"/>
+      <c r="K15" s="52"/>
+      <c r="L15" s="52"/>
+      <c r="M15" s="52"/>
+      <c r="N15" s="52"/>
+      <c r="O15" s="53"/>
       <c r="Q15" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="R15" s="49" t="s">
+      <c r="R15" s="58" t="s">
         <v>40</v>
       </c>
       <c r="S15" s="44"/>
       <c r="T15" s="45"/>
     </row>
     <row r="16" spans="2:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I16" s="55"/>
-      <c r="J16" s="56"/>
-      <c r="K16" s="56"/>
-      <c r="L16" s="56"/>
-      <c r="M16" s="56"/>
-      <c r="N16" s="56"/>
-      <c r="O16" s="57"/>
+      <c r="I16" s="51"/>
+      <c r="J16" s="52"/>
+      <c r="K16" s="52"/>
+      <c r="L16" s="52"/>
+      <c r="M16" s="52"/>
+      <c r="N16" s="52"/>
+      <c r="O16" s="53"/>
       <c r="Q16" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="R16" s="50" t="s">
+      <c r="R16" s="46" t="s">
         <v>42</v>
       </c>
       <c r="S16" s="44"/>
       <c r="T16" s="45"/>
     </row>
     <row r="17" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I17" s="55"/>
-      <c r="J17" s="56"/>
-      <c r="K17" s="56"/>
-      <c r="L17" s="56"/>
-      <c r="M17" s="56"/>
-      <c r="N17" s="56"/>
-      <c r="O17" s="57"/>
+      <c r="I17" s="51"/>
+      <c r="J17" s="52"/>
+      <c r="K17" s="52"/>
+      <c r="L17" s="52"/>
+      <c r="M17" s="52"/>
+      <c r="N17" s="52"/>
+      <c r="O17" s="53"/>
       <c r="Q17" s="5" t="s">
         <v>43</v>
       </c>
-      <c r="R17" s="50" t="s">
+      <c r="R17" s="46" t="s">
         <v>44</v>
       </c>
       <c r="S17" s="44"/>
       <c r="T17" s="45"/>
     </row>
     <row r="18" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I18" s="55"/>
-      <c r="J18" s="56"/>
-      <c r="K18" s="56"/>
-      <c r="L18" s="56"/>
-      <c r="M18" s="56"/>
-      <c r="N18" s="56"/>
-      <c r="O18" s="57"/>
+      <c r="I18" s="51"/>
+      <c r="J18" s="52"/>
+      <c r="K18" s="52"/>
+      <c r="L18" s="52"/>
+      <c r="M18" s="52"/>
+      <c r="N18" s="52"/>
+      <c r="O18" s="53"/>
       <c r="Q18" s="5" t="s">
         <v>45</v>
       </c>
-      <c r="R18" s="50" t="s">
+      <c r="R18" s="46" t="s">
         <v>46</v>
       </c>
       <c r="S18" s="44"/>
       <c r="T18" s="45"/>
     </row>
     <row r="19" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I19" s="55"/>
-      <c r="J19" s="56"/>
-      <c r="K19" s="56"/>
-      <c r="L19" s="56"/>
-      <c r="M19" s="56"/>
-      <c r="N19" s="56"/>
-      <c r="O19" s="57"/>
+      <c r="I19" s="51"/>
+      <c r="J19" s="52"/>
+      <c r="K19" s="52"/>
+      <c r="L19" s="52"/>
+      <c r="M19" s="52"/>
+      <c r="N19" s="52"/>
+      <c r="O19" s="53"/>
       <c r="Q19" s="5" t="s">
         <v>47</v>
       </c>
-      <c r="R19" s="50" t="s">
+      <c r="R19" s="46" t="s">
         <v>48</v>
       </c>
       <c r="S19" s="44"/>
       <c r="T19" s="45"/>
     </row>
     <row r="20" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I20" s="55"/>
-      <c r="J20" s="56"/>
-      <c r="K20" s="56"/>
-      <c r="L20" s="56"/>
-      <c r="M20" s="56"/>
-      <c r="N20" s="56"/>
-      <c r="O20" s="57"/>
+      <c r="I20" s="51"/>
+      <c r="J20" s="52"/>
+      <c r="K20" s="52"/>
+      <c r="L20" s="52"/>
+      <c r="M20" s="52"/>
+      <c r="N20" s="52"/>
+      <c r="O20" s="53"/>
       <c r="Q20" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="R20" s="50" t="s">
+      <c r="R20" s="46" t="s">
         <v>50</v>
       </c>
       <c r="S20" s="44"/>
       <c r="T20" s="45"/>
     </row>
     <row r="21" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I21" s="55"/>
-      <c r="J21" s="56"/>
-      <c r="K21" s="56"/>
-      <c r="L21" s="56"/>
-      <c r="M21" s="56"/>
-      <c r="N21" s="56"/>
-      <c r="O21" s="57"/>
+      <c r="I21" s="51"/>
+      <c r="J21" s="52"/>
+      <c r="K21" s="52"/>
+      <c r="L21" s="52"/>
+      <c r="M21" s="52"/>
+      <c r="N21" s="52"/>
+      <c r="O21" s="53"/>
       <c r="Q21" s="5" t="s">
         <v>51</v>
       </c>
-      <c r="R21" s="50" t="s">
+      <c r="R21" s="46" t="s">
         <v>52</v>
       </c>
       <c r="S21" s="44"/>
       <c r="T21" s="45"/>
     </row>
     <row r="22" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I22" s="55"/>
-      <c r="J22" s="56"/>
-      <c r="K22" s="56"/>
-      <c r="L22" s="56"/>
-      <c r="M22" s="56"/>
-      <c r="N22" s="56"/>
-      <c r="O22" s="57"/>
+      <c r="I22" s="51"/>
+      <c r="J22" s="52"/>
+      <c r="K22" s="52"/>
+      <c r="L22" s="52"/>
+      <c r="M22" s="52"/>
+      <c r="N22" s="52"/>
+      <c r="O22" s="53"/>
     </row>
     <row r="23" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I23" s="55"/>
-      <c r="J23" s="56"/>
-      <c r="K23" s="56"/>
-      <c r="L23" s="56"/>
-      <c r="M23" s="56"/>
-      <c r="N23" s="56"/>
-      <c r="O23" s="57"/>
+      <c r="I23" s="51"/>
+      <c r="J23" s="52"/>
+      <c r="K23" s="52"/>
+      <c r="L23" s="52"/>
+      <c r="M23" s="52"/>
+      <c r="N23" s="52"/>
+      <c r="O23" s="53"/>
     </row>
     <row r="24" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="I24" s="58"/>
-      <c r="J24" s="59"/>
-      <c r="K24" s="59"/>
-      <c r="L24" s="59"/>
-      <c r="M24" s="59"/>
-      <c r="N24" s="59"/>
-      <c r="O24" s="60"/>
+      <c r="I24" s="54"/>
+      <c r="J24" s="55"/>
+      <c r="K24" s="55"/>
+      <c r="L24" s="55"/>
+      <c r="M24" s="55"/>
+      <c r="N24" s="55"/>
+      <c r="O24" s="56"/>
     </row>
     <row r="25" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="26" spans="9:20" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5458,6 +5451,21 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="24">
+    <mergeCell ref="D1:I1"/>
+    <mergeCell ref="B3:K3"/>
+    <mergeCell ref="B6:E6"/>
+    <mergeCell ref="I6:O6"/>
+    <mergeCell ref="Q6:T6"/>
+    <mergeCell ref="C8:E8"/>
+    <mergeCell ref="C9:E9"/>
+    <mergeCell ref="R17:T17"/>
+    <mergeCell ref="R18:T18"/>
+    <mergeCell ref="R19:T19"/>
+    <mergeCell ref="C10:E10"/>
+    <mergeCell ref="C11:E11"/>
+    <mergeCell ref="C12:E12"/>
+    <mergeCell ref="C13:E13"/>
+    <mergeCell ref="C14:E14"/>
     <mergeCell ref="R20:T20"/>
     <mergeCell ref="Q8:S8"/>
     <mergeCell ref="Q9:S9"/>
@@ -5467,21 +5475,6 @@
     <mergeCell ref="R15:T15"/>
     <mergeCell ref="R16:T16"/>
     <mergeCell ref="R21:T21"/>
-    <mergeCell ref="C8:E8"/>
-    <mergeCell ref="C9:E9"/>
-    <mergeCell ref="R17:T17"/>
-    <mergeCell ref="R18:T18"/>
-    <mergeCell ref="R19:T19"/>
-    <mergeCell ref="D1:I1"/>
-    <mergeCell ref="B3:K3"/>
-    <mergeCell ref="B6:E6"/>
-    <mergeCell ref="I6:O6"/>
-    <mergeCell ref="Q6:T6"/>
-    <mergeCell ref="C10:E10"/>
-    <mergeCell ref="C11:E11"/>
-    <mergeCell ref="C12:E12"/>
-    <mergeCell ref="C13:E13"/>
-    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -5496,8 +5489,8 @@
   </sheetPr>
   <dimension ref="B1:AB1002"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView topLeftCell="A4" zoomScale="78" workbookViewId="0">
+      <selection activeCell="E12" sqref="E12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -5543,7 +5536,7 @@
     </row>
     <row r="2" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="66" t="s">
+      <c r="B3" s="61" t="s">
         <v>53</v>
       </c>
       <c r="C3" s="44"/>
@@ -5554,7 +5547,7 @@
     <row r="4" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="5" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B5" s="9" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
     </row>
     <row r="6" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -5566,16 +5559,16 @@
       <c r="B7" s="16"/>
     </row>
     <row r="8" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B8" s="67" t="s">
+      <c r="B8" s="62" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="67" t="s">
+      <c r="C8" s="62" t="s">
         <v>56</v>
       </c>
-      <c r="D8" s="67" t="s">
+      <c r="D8" s="62" t="s">
         <v>57</v>
       </c>
-      <c r="E8" s="70" t="s">
+      <c r="E8" s="66" t="s">
         <v>58</v>
       </c>
       <c r="F8" s="44"/>
@@ -5603,13 +5596,13 @@
       <c r="AB8" s="45"/>
     </row>
     <row r="9" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B9" s="68"/>
-      <c r="C9" s="62"/>
-      <c r="D9" s="62"/>
-      <c r="E9" s="69" t="s">
+      <c r="B9" s="63"/>
+      <c r="C9" s="64"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="65" t="s">
         <v>59</v>
       </c>
-      <c r="F9" s="65" t="s">
+      <c r="F9" s="68" t="s">
         <v>60</v>
       </c>
       <c r="G9" s="44"/>
@@ -5621,7 +5614,7 @@
       <c r="M9" s="44"/>
       <c r="N9" s="44"/>
       <c r="O9" s="45"/>
-      <c r="P9" s="63" t="s">
+      <c r="P9" s="71" t="s">
         <v>61</v>
       </c>
       <c r="Q9" s="44"/>
@@ -5629,7 +5622,7 @@
       <c r="S9" s="44"/>
       <c r="T9" s="44"/>
       <c r="U9" s="45"/>
-      <c r="V9" s="64" t="s">
+      <c r="V9" s="72" t="s">
         <v>62</v>
       </c>
       <c r="W9" s="44"/>
@@ -5640,15 +5633,15 @@
       <c r="AB9" s="45"/>
     </row>
     <row r="10" spans="2:28" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B10" s="68"/>
-      <c r="C10" s="71" t="s">
+      <c r="B10" s="63"/>
+      <c r="C10" s="67" t="s">
         <v>63</v>
       </c>
-      <c r="D10" s="71" t="s">
+      <c r="D10" s="67" t="s">
         <v>64</v>
       </c>
-      <c r="E10" s="68"/>
-      <c r="F10" s="65" t="s">
+      <c r="E10" s="63"/>
+      <c r="F10" s="68" t="s">
         <v>65</v>
       </c>
       <c r="G10" s="45"/>
@@ -5656,63 +5649,63 @@
         <v>66</v>
       </c>
       <c r="I10" s="45"/>
-      <c r="J10" s="65" t="s">
+      <c r="J10" s="68" t="s">
         <v>67</v>
       </c>
       <c r="K10" s="45"/>
-      <c r="L10" s="65" t="s">
+      <c r="L10" s="68" t="s">
         <v>68</v>
       </c>
       <c r="M10" s="45"/>
-      <c r="N10" s="65" t="s">
+      <c r="N10" s="68" t="s">
         <v>69</v>
       </c>
       <c r="O10" s="45"/>
-      <c r="P10" s="72" t="s">
+      <c r="P10" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="Q10" s="72" t="s">
+      <c r="Q10" s="69" t="s">
         <v>43</v>
       </c>
-      <c r="R10" s="72" t="s">
+      <c r="R10" s="69" t="s">
         <v>45</v>
       </c>
-      <c r="S10" s="72" t="s">
+      <c r="S10" s="69" t="s">
         <v>47</v>
       </c>
-      <c r="T10" s="72" t="s">
+      <c r="T10" s="69" t="s">
         <v>49</v>
       </c>
-      <c r="U10" s="72" t="s">
+      <c r="U10" s="69" t="s">
         <v>51</v>
       </c>
-      <c r="V10" s="61">
+      <c r="V10" s="70">
         <v>0</v>
       </c>
-      <c r="W10" s="61">
+      <c r="W10" s="70">
         <v>1</v>
       </c>
-      <c r="X10" s="61">
+      <c r="X10" s="70">
         <v>2</v>
       </c>
-      <c r="Y10" s="61" t="s">
+      <c r="Y10" s="70" t="s">
         <v>70</v>
       </c>
-      <c r="Z10" s="61" t="s">
+      <c r="Z10" s="70" t="s">
         <v>71</v>
       </c>
-      <c r="AA10" s="61" t="s">
+      <c r="AA10" s="70" t="s">
         <v>72</v>
       </c>
-      <c r="AB10" s="61" t="s">
+      <c r="AB10" s="70" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="11" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B11" s="62"/>
-      <c r="C11" s="62"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="62"/>
+      <c r="B11" s="64"/>
+      <c r="C11" s="64"/>
+      <c r="D11" s="64"/>
+      <c r="E11" s="64"/>
       <c r="F11" s="17" t="s">
         <v>74</v>
       </c>
@@ -5743,19 +5736,19 @@
       <c r="O11" s="17" t="s">
         <v>75</v>
       </c>
-      <c r="P11" s="62"/>
-      <c r="Q11" s="62"/>
-      <c r="R11" s="62"/>
-      <c r="S11" s="62"/>
-      <c r="T11" s="62"/>
-      <c r="U11" s="62"/>
-      <c r="V11" s="62"/>
-      <c r="W11" s="62"/>
-      <c r="X11" s="62"/>
-      <c r="Y11" s="62"/>
-      <c r="Z11" s="62"/>
-      <c r="AA11" s="62"/>
-      <c r="AB11" s="62"/>
+      <c r="P11" s="64"/>
+      <c r="Q11" s="64"/>
+      <c r="R11" s="64"/>
+      <c r="S11" s="64"/>
+      <c r="T11" s="64"/>
+      <c r="U11" s="64"/>
+      <c r="V11" s="64"/>
+      <c r="W11" s="64"/>
+      <c r="X11" s="64"/>
+      <c r="Y11" s="64"/>
+      <c r="Z11" s="64"/>
+      <c r="AA11" s="64"/>
+      <c r="AB11" s="64"/>
     </row>
     <row r="12" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="18" t="s">
@@ -5765,35 +5758,35 @@
         <v>77</v>
       </c>
       <c r="D12" s="19" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="E12" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="F12" s="21" t="s">
         <v>79</v>
       </c>
-      <c r="F12" s="21" t="s">
-        <v>80</v>
-      </c>
       <c r="G12" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I12" s="21"/>
       <c r="J12" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K12" s="21"/>
       <c r="L12" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="M12" s="21"/>
       <c r="N12" s="21"/>
       <c r="O12" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P12" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Q12" s="22"/>
       <c r="R12" s="22"/>
@@ -5802,60 +5795,60 @@
       <c r="U12" s="22"/>
       <c r="V12" s="23"/>
       <c r="W12" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="X12" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Y12" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="Z12" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA12" s="23"/>
       <c r="AB12" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="13" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B13" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="C13" s="18" t="s">
         <v>81</v>
       </c>
-      <c r="C13" s="18" t="s">
+      <c r="D13" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="E13" s="20" t="s">
         <v>82</v>
       </c>
-      <c r="D13" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="E13" s="20" t="s">
-        <v>84</v>
-      </c>
       <c r="F13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I13" s="21"/>
       <c r="J13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="K13" s="21"/>
       <c r="L13" s="21"/>
       <c r="M13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N13" s="21"/>
       <c r="O13" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P13" s="22"/>
       <c r="Q13" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="R13" s="22"/>
       <c r="S13" s="22"/>
@@ -5866,50 +5859,50 @@
       <c r="X13" s="23"/>
       <c r="Y13" s="23"/>
       <c r="Z13" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA13" s="23"/>
       <c r="AB13" s="23"/>
     </row>
     <row r="14" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B14" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="C14" s="18" t="s">
+        <v>84</v>
+      </c>
+      <c r="D14" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>85</v>
       </c>
-      <c r="C14" s="18" t="s">
-        <v>86</v>
-      </c>
-      <c r="D14" s="19" t="s">
-        <v>139</v>
-      </c>
-      <c r="E14" s="20" t="s">
-        <v>88</v>
-      </c>
       <c r="F14" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G14" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="I14" s="21"/>
       <c r="J14" s="21"/>
       <c r="K14" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L14" s="21"/>
       <c r="M14" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N14" s="21"/>
       <c r="O14" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="P14" s="22"/>
       <c r="Q14" s="22"/>
       <c r="R14" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="S14" s="22"/>
       <c r="T14" s="22"/>
@@ -5919,51 +5912,51 @@
       <c r="X14" s="23"/>
       <c r="Y14" s="23"/>
       <c r="Z14" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA14" s="23"/>
       <c r="AB14" s="23"/>
     </row>
     <row r="15" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B15" s="18" t="s">
+        <v>86</v>
+      </c>
+      <c r="C15" s="18" t="s">
+        <v>87</v>
+      </c>
+      <c r="D15" s="19" t="s">
+        <v>88</v>
+      </c>
+      <c r="E15" s="20" t="s">
         <v>89</v>
       </c>
-      <c r="C15" s="18" t="s">
-        <v>90</v>
-      </c>
-      <c r="D15" s="19" t="s">
-        <v>91</v>
-      </c>
-      <c r="E15" s="20" t="s">
-        <v>92</v>
-      </c>
       <c r="F15" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H15" s="21"/>
       <c r="I15" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="J15" s="21"/>
       <c r="K15" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="L15" s="21"/>
       <c r="M15" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="N15" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O15" s="21"/>
       <c r="P15" s="22"/>
       <c r="Q15" s="22"/>
       <c r="R15" s="22"/>
       <c r="S15" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="T15" s="22"/>
       <c r="U15" s="22"/>
@@ -5972,27 +5965,27 @@
       <c r="X15" s="23"/>
       <c r="Y15" s="23"/>
       <c r="Z15" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="AA15" s="23"/>
       <c r="AB15" s="23"/>
     </row>
     <row r="16" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="18" t="s">
+        <v>90</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>91</v>
+      </c>
+      <c r="D16" s="19" t="s">
+        <v>92</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>93</v>
-      </c>
-      <c r="C16" s="18" t="s">
-        <v>94</v>
-      </c>
-      <c r="D16" s="19" t="s">
-        <v>95</v>
-      </c>
-      <c r="E16" s="20" t="s">
-        <v>96</v>
       </c>
       <c r="F16" s="21"/>
       <c r="G16" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H16" s="21"/>
       <c r="I16" s="21"/>
@@ -6001,7 +5994,7 @@
       <c r="L16" s="21"/>
       <c r="M16" s="21"/>
       <c r="N16" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="O16" s="21"/>
       <c r="P16" s="22"/>
@@ -6009,11 +6002,11 @@
       <c r="R16" s="22"/>
       <c r="S16" s="22"/>
       <c r="T16" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="U16" s="22"/>
       <c r="V16" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W16" s="23"/>
       <c r="X16" s="23"/>
@@ -6024,20 +6017,20 @@
     </row>
     <row r="17" spans="2:28" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B17" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D17" s="19" t="s">
+        <v>96</v>
+      </c>
+      <c r="E17" s="20" t="s">
         <v>97</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>98</v>
-      </c>
-      <c r="D17" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="E17" s="20" t="s">
-        <v>100</v>
       </c>
       <c r="F17" s="21"/>
       <c r="G17" s="21" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="H17" s="21"/>
       <c r="I17" s="21"/>
@@ -6053,10 +6046,10 @@
       <c r="S17" s="22"/>
       <c r="T17" s="22"/>
       <c r="U17" s="22" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="V17" s="23" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="W17" s="23"/>
       <c r="X17" s="23"/>
@@ -7054,6 +7047,20 @@
     <row r="1002" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="30">
+    <mergeCell ref="AA10:AA11"/>
+    <mergeCell ref="P9:U9"/>
+    <mergeCell ref="V9:AB9"/>
+    <mergeCell ref="F9:O9"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="AB10:AB11"/>
+    <mergeCell ref="T10:T11"/>
+    <mergeCell ref="U10:U11"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="V10:V11"/>
+    <mergeCell ref="W10:W11"/>
+    <mergeCell ref="X10:X11"/>
+    <mergeCell ref="Y10:Y11"/>
+    <mergeCell ref="Z10:Z11"/>
     <mergeCell ref="D1:G1"/>
     <mergeCell ref="B3:F3"/>
     <mergeCell ref="B8:B11"/>
@@ -7070,20 +7077,6 @@
     <mergeCell ref="Q10:Q11"/>
     <mergeCell ref="R10:R11"/>
     <mergeCell ref="S10:S11"/>
-    <mergeCell ref="AA10:AA11"/>
-    <mergeCell ref="P9:U9"/>
-    <mergeCell ref="V9:AB9"/>
-    <mergeCell ref="F9:O9"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="AB10:AB11"/>
-    <mergeCell ref="T10:T11"/>
-    <mergeCell ref="U10:U11"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="V10:V11"/>
-    <mergeCell ref="W10:W11"/>
-    <mergeCell ref="X10:X11"/>
-    <mergeCell ref="Y10:Y11"/>
-    <mergeCell ref="Z10:Z11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -7097,8 +7090,8 @@
   </sheetPr>
   <dimension ref="B1:N1000"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+    <sheetView tabSelected="1" zoomScale="63" workbookViewId="0">
+      <selection activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.45"/>
@@ -7130,8 +7123,8 @@
     </row>
     <row r="2" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
     <row r="3" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B3" s="84" t="s">
-        <v>101</v>
+      <c r="B3" s="98" t="s">
+        <v>98</v>
       </c>
       <c r="C3" s="44"/>
       <c r="D3" s="44"/>
@@ -7145,174 +7138,174 @@
       <c r="L3" s="45"/>
     </row>
     <row r="4" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B4" s="85" t="s">
+      <c r="B4" s="99" t="s">
+        <v>99</v>
+      </c>
+      <c r="C4" s="76" t="s">
+        <v>100</v>
+      </c>
+      <c r="D4" s="101" t="s">
+        <v>101</v>
+      </c>
+      <c r="E4" s="103" t="s">
         <v>102</v>
-      </c>
-      <c r="C4" s="89" t="s">
-        <v>103</v>
-      </c>
-      <c r="D4" s="87" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="80" t="s">
-        <v>105</v>
       </c>
       <c r="F4" s="44"/>
       <c r="G4" s="44"/>
       <c r="H4" s="44"/>
       <c r="I4" s="44"/>
       <c r="J4" s="45"/>
-      <c r="K4" s="80" t="s">
-        <v>106</v>
+      <c r="K4" s="103" t="s">
+        <v>103</v>
       </c>
       <c r="L4" s="45"/>
     </row>
     <row r="5" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B5" s="86"/>
-      <c r="C5" s="90"/>
-      <c r="D5" s="88"/>
+      <c r="B5" s="100"/>
+      <c r="C5" s="86"/>
+      <c r="D5" s="102"/>
       <c r="E5" s="25" t="s">
-        <v>107</v>
-      </c>
-      <c r="F5" s="81" t="s">
+        <v>104</v>
+      </c>
+      <c r="F5" s="95" t="s">
         <v>63</v>
       </c>
-      <c r="G5" s="82"/>
-      <c r="H5" s="82"/>
-      <c r="I5" s="82"/>
-      <c r="J5" s="83"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="96"/>
+      <c r="I5" s="96"/>
+      <c r="J5" s="97"/>
       <c r="K5" s="25" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="L5" s="25" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B6" s="26">
         <v>11</v>
       </c>
-      <c r="C6" s="91" t="s">
-        <v>110</v>
+      <c r="C6" s="84" t="s">
+        <v>107</v>
       </c>
       <c r="D6" s="27" t="s">
         <v>76</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="F6" s="79" t="s">
-        <v>111</v>
-      </c>
-      <c r="G6" s="59"/>
-      <c r="H6" s="59"/>
-      <c r="I6" s="59"/>
-      <c r="J6" s="60"/>
+        <v>137</v>
+      </c>
+      <c r="F6" s="106" t="s">
+        <v>108</v>
+      </c>
+      <c r="G6" s="55"/>
+      <c r="H6" s="55"/>
+      <c r="I6" s="55"/>
+      <c r="J6" s="56"/>
       <c r="K6" s="28" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
       <c r="L6" s="28" t="s">
-        <v>78</v>
+        <v>134</v>
       </c>
     </row>
     <row r="7" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B7" s="26">
         <v>12</v>
       </c>
-      <c r="C7" s="92"/>
+      <c r="C7" s="85"/>
       <c r="D7" s="27" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="E7" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="F7" s="80" t="s">
-        <v>112</v>
+        <v>137</v>
+      </c>
+      <c r="F7" s="103" t="s">
+        <v>109</v>
       </c>
       <c r="G7" s="44"/>
       <c r="H7" s="44"/>
       <c r="I7" s="44"/>
       <c r="J7" s="45"/>
       <c r="K7" s="26" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
       <c r="L7" s="26" t="s">
-        <v>83</v>
+        <v>135</v>
       </c>
     </row>
     <row r="8" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B8" s="26">
         <v>13</v>
       </c>
-      <c r="C8" s="92"/>
+      <c r="C8" s="85"/>
       <c r="D8" s="29" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E8" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="F8" s="80" t="s">
-        <v>113</v>
+        <v>137</v>
+      </c>
+      <c r="F8" s="103" t="s">
+        <v>110</v>
       </c>
       <c r="G8" s="44"/>
       <c r="H8" s="44"/>
       <c r="I8" s="44"/>
       <c r="J8" s="45"/>
       <c r="K8" s="26" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
       <c r="L8" s="26" t="s">
-        <v>87</v>
+        <v>136</v>
       </c>
     </row>
     <row r="9" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B9" s="26">
         <v>14</v>
       </c>
-      <c r="C9" s="92"/>
+      <c r="C9" s="85"/>
       <c r="D9" s="29" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>140</v>
-      </c>
-      <c r="F9" s="80" t="s">
-        <v>114</v>
+        <v>137</v>
+      </c>
+      <c r="F9" s="103" t="s">
+        <v>111</v>
       </c>
       <c r="G9" s="44"/>
       <c r="H9" s="44"/>
       <c r="I9" s="44"/>
       <c r="J9" s="45"/>
       <c r="K9" s="30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L9" s="30" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="10" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B10" s="25">
         <v>15</v>
       </c>
-      <c r="C10" s="90"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="29" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
       <c r="E10" s="25" t="s">
-        <v>116</v>
-      </c>
-      <c r="F10" s="81" t="s">
-        <v>117</v>
-      </c>
-      <c r="G10" s="82"/>
-      <c r="H10" s="82"/>
-      <c r="I10" s="82"/>
-      <c r="J10" s="83"/>
+        <v>113</v>
+      </c>
+      <c r="F10" s="95" t="s">
+        <v>114</v>
+      </c>
+      <c r="G10" s="96"/>
+      <c r="H10" s="96"/>
+      <c r="I10" s="96"/>
+      <c r="J10" s="97"/>
       <c r="K10" s="31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
       <c r="L10" s="31" t="s">
-        <v>115</v>
+        <v>112</v>
       </c>
     </row>
     <row r="11" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
@@ -7330,88 +7323,88 @@
     </row>
     <row r="12" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B12" s="32" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="K12" s="33"/>
     </row>
     <row r="13" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B13" s="74" t="s">
+      <c r="B13" s="87" t="s">
+        <v>116</v>
+      </c>
+      <c r="C13" s="88"/>
+      <c r="D13" s="88"/>
+      <c r="E13" s="89"/>
+      <c r="F13" s="90" t="s">
+        <v>117</v>
+      </c>
+      <c r="G13" s="91"/>
+      <c r="H13" s="87" t="s">
+        <v>118</v>
+      </c>
+      <c r="I13" s="88"/>
+      <c r="J13" s="88"/>
+      <c r="K13" s="88"/>
+      <c r="L13" s="104"/>
+      <c r="M13" s="105" t="s">
         <v>119</v>
       </c>
-      <c r="C13" s="75"/>
-      <c r="D13" s="75"/>
-      <c r="E13" s="93"/>
-      <c r="F13" s="94" t="s">
-        <v>120</v>
-      </c>
-      <c r="G13" s="78"/>
-      <c r="H13" s="74" t="s">
-        <v>121</v>
-      </c>
-      <c r="I13" s="75"/>
-      <c r="J13" s="75"/>
-      <c r="K13" s="75"/>
-      <c r="L13" s="76"/>
-      <c r="M13" s="77" t="s">
-        <v>122</v>
-      </c>
-      <c r="N13" s="78"/>
+      <c r="N13" s="91"/>
     </row>
     <row r="14" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B14" s="95" t="s">
+      <c r="B14" s="92" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="81" t="s">
+        <v>121</v>
+      </c>
+      <c r="D14" s="81" t="s">
+        <v>122</v>
+      </c>
+      <c r="E14" s="78" t="s">
         <v>123</v>
       </c>
-      <c r="C14" s="97" t="s">
+      <c r="F14" s="79" t="s">
         <v>124</v>
       </c>
-      <c r="D14" s="97" t="s">
+      <c r="G14" s="93" t="s">
         <v>125</v>
       </c>
-      <c r="E14" s="102" t="s">
+      <c r="H14" s="80" t="s">
         <v>126</v>
       </c>
-      <c r="F14" s="103" t="s">
+      <c r="I14" s="81" t="s">
+        <v>120</v>
+      </c>
+      <c r="J14" s="81" t="s">
         <v>127</v>
       </c>
-      <c r="G14" s="98" t="s">
+      <c r="K14" s="82" t="s">
         <v>128</v>
       </c>
-      <c r="H14" s="104" t="s">
+      <c r="L14" s="83" t="s">
         <v>129</v>
       </c>
-      <c r="I14" s="97" t="s">
-        <v>123</v>
-      </c>
-      <c r="J14" s="97" t="s">
+      <c r="M14" s="74" t="s">
         <v>130</v>
       </c>
-      <c r="K14" s="105" t="s">
+      <c r="N14" s="76" t="s">
         <v>131</v>
-      </c>
-      <c r="L14" s="106" t="s">
-        <v>132</v>
-      </c>
-      <c r="M14" s="100" t="s">
-        <v>133</v>
-      </c>
-      <c r="N14" s="89" t="s">
-        <v>134</v>
       </c>
     </row>
     <row r="15" spans="2:14" ht="15" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B15" s="96"/>
-      <c r="C15" s="62"/>
-      <c r="D15" s="62"/>
-      <c r="E15" s="62"/>
-      <c r="F15" s="101"/>
-      <c r="G15" s="99"/>
-      <c r="H15" s="96"/>
-      <c r="I15" s="62"/>
-      <c r="J15" s="62"/>
-      <c r="K15" s="58"/>
-      <c r="L15" s="101"/>
-      <c r="M15" s="96"/>
-      <c r="N15" s="101"/>
+      <c r="B15" s="75"/>
+      <c r="C15" s="64"/>
+      <c r="D15" s="64"/>
+      <c r="E15" s="64"/>
+      <c r="F15" s="77"/>
+      <c r="G15" s="94"/>
+      <c r="H15" s="75"/>
+      <c r="I15" s="64"/>
+      <c r="J15" s="64"/>
+      <c r="K15" s="54"/>
+      <c r="L15" s="77"/>
+      <c r="M15" s="75"/>
+      <c r="N15" s="77"/>
     </row>
     <row r="16" spans="2:14" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
       <c r="B16" s="6">
@@ -7430,10 +7423,10 @@
         <v>0</v>
       </c>
       <c r="G16" s="37" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="H16" s="38" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="I16" s="6">
         <f>SUM(J16:K16)</f>
@@ -7449,7 +7442,7 @@
         <v>100</v>
       </c>
       <c r="M16" s="41" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="N16" s="42">
         <v>0</v>
@@ -8441,6 +8434,28 @@
     <row r="1000" ht="14.25" customHeight="1" x14ac:dyDescent="0.45"/>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="H13:L13"/>
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="F6:J6"/>
+    <mergeCell ref="F7:J7"/>
+    <mergeCell ref="F8:J8"/>
+    <mergeCell ref="F9:J9"/>
+    <mergeCell ref="F10:J10"/>
+    <mergeCell ref="F5:J5"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="B3:L3"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="D4:D5"/>
+    <mergeCell ref="E4:J4"/>
+    <mergeCell ref="K4:L4"/>
+    <mergeCell ref="C4:C5"/>
+    <mergeCell ref="C6:C10"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="F13:G13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="C14:C15"/>
+    <mergeCell ref="D14:D15"/>
+    <mergeCell ref="G14:G15"/>
     <mergeCell ref="M14:M15"/>
     <mergeCell ref="N14:N15"/>
     <mergeCell ref="E14:E15"/>
@@ -8450,28 +8465,6 @@
     <mergeCell ref="J14:J15"/>
     <mergeCell ref="K14:K15"/>
     <mergeCell ref="L14:L15"/>
-    <mergeCell ref="C6:C10"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="F13:G13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="D14:D15"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F5:J5"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="B3:L3"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="D4:D5"/>
-    <mergeCell ref="E4:J4"/>
-    <mergeCell ref="K4:L4"/>
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="H13:L13"/>
-    <mergeCell ref="M13:N13"/>
-    <mergeCell ref="F6:J6"/>
-    <mergeCell ref="F7:J7"/>
-    <mergeCell ref="F8:J8"/>
-    <mergeCell ref="F9:J9"/>
-    <mergeCell ref="F10:J10"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait"/>

</xml_diff>